<commit_message>
Edit adding data to scenario
</commit_message>
<xml_diff>
--- a/src/NamedRangeTestApp/Data/testSet/scenario.xlsx
+++ b/src/NamedRangeTestApp/Data/testSet/scenario.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\NamedRangeTestApp\NamedRangeTestApp\Data\testSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evgeny\Desktop\testNamedRange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47ACC450-7B54-492E-9255-ECEB4496E269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED3B50C-89FE-47E6-9C5C-E101107696FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30765" yWindow="1005" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="general_collumn_cells">'general'!$C$4:$C$9</definedName>
-    <definedName name="general_row_cells">'general'!$C$11:$G$11</definedName>
-    <definedName name="general_single_cell">'general'!$C$2</definedName>
-    <definedName name="general_table_cells">'general'!$C$13:$G$16</definedName>
+    <definedName name="general_column_cells">general!$C$4:$C$9</definedName>
+    <definedName name="general_row_cells">general!$C$11:$G$11</definedName>
+    <definedName name="general_single_cell">general!$C$2</definedName>
+    <definedName name="general_table_cells">general!$C$13:$G$16</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,24 +41,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>general_single_cell</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>general_collumn_cells</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
   <si>
     <t>general_row_cells</t>
@@ -67,27 +52,14 @@
     <t>general_table_cells</t>
   </si>
   <si>
-    <t>6748</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>qwe</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>general_column_cells</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,7 +82,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,51 +105,25 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,142 +406,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G16"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1" style="3"/>
-    <col min="2" max="2" width="27" customWidth="1" style="3"/>
-    <col min="3" max="3" width="9.140625" customWidth="1" style="3"/>
-    <col min="4" max="16384" width="9.140625" customWidth="1" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="27" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
     </row>
-    <row r="4">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="5"/>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="5"/>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="5"/>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="5"/>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="5"/>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="7"/>
-      <c r="C14" s="2" t="s">
+      <c r="C11" s="2">
         <v>8</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
         <v>10</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F11" s="2">
         <v>11</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G11" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="7"/>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2">
+        <v>16</v>
+      </c>
+      <c r="G13" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="2">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>21</v>
+      </c>
+      <c r="G14" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="2">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2">
+        <v>25</v>
+      </c>
+      <c r="F15" s="2">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="2">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2">
+        <v>30</v>
+      </c>
+      <c r="F16" s="2">
+        <v>31</v>
+      </c>
+      <c r="G16" s="2">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="2">
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added inserting of values from scenario to calc
</commit_message>
<xml_diff>
--- a/src/NamedRangeTestApp/Data/testSet/scenario.xlsx
+++ b/src/NamedRangeTestApp/Data/testSet/scenario.xlsx
@@ -16,12 +16,12 @@
     <sheet name="general" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="general_column_cells">general!$C$4:$C$9</definedName>
-    <definedName name="general_row_cells">general!$C$11:$G$11</definedName>
-    <definedName name="general_single_cell">general!$C$2</definedName>
-    <definedName name="general_table_cells">general!$C$13:$G$16</definedName>
+    <definedName name="general_column_cells">'general'!$C$4:$C$9</definedName>
+    <definedName name="general_row_cells">'general'!$C$11:$G$11</definedName>
+    <definedName name="general_single_cell">'general'!$C$2</definedName>
+    <definedName name="general_table_cells">'general'!$C$13:$G$16</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,20 +46,21 @@
     <t>general_single_cell</t>
   </si>
   <si>
+    <t>general_column_cells</t>
+  </si>
+  <si>
     <t>general_row_cells</t>
   </si>
   <si>
     <t>general_table_cells</t>
-  </si>
-  <si>
-    <t>general_column_cells</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,20 +111,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -406,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G16"/>
+  <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B9"/>
@@ -414,12 +415,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="27" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" style="3"/>
+    <col min="2" max="2" width="27" customWidth="1" style="3"/>
+    <col min="3" max="16384" width="9.140625" customWidth="1" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,69 +428,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="B5" s="5"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="B6" s="5"/>
       <c r="C6" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="B7" s="5"/>
       <c r="C7" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="B8" s="5"/>
       <c r="C8" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="B9" s="5"/>
       <c r="C9" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
         <v>8</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
         <v>10</v>
       </c>
-      <c r="F11" s="2">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13">
       <c r="B13" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
         <v>13</v>
@@ -507,7 +508,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="B14" s="5"/>
       <c r="C14" s="2">
         <v>18</v>
@@ -523,7 +524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="B15" s="5"/>
       <c r="C15" s="2">
         <v>23</v>
@@ -541,7 +542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="B16" s="5"/>
       <c r="C16" s="2">
         <v>28</v>
@@ -560,10 +561,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells>
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new named ranges results
</commit_message>
<xml_diff>
--- a/src/NamedRangeTestApp/Data/testSet/scenario.xlsx
+++ b/src/NamedRangeTestApp/Data/testSet/scenario.xlsx
@@ -425,7 +425,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -436,35 +436,37 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="5"/>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="5"/>
       <c r="C6" s="2">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="5"/>
       <c r="C7" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="5"/>
       <c r="C8" s="2">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="5"/>
       <c r="C9" s="2">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
@@ -475,17 +477,19 @@
         <v>2</v>
       </c>
       <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
         <v>3</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
         <v>5</v>
       </c>
-      <c r="E11" s="2">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">

</xml_diff>